<commit_message>
jane push file 1/10/2024 4:12 pm
</commit_message>
<xml_diff>
--- a/CASUAL/LA CHO/ENRIQUEZ, ANABEL ORTEGA.xlsx
+++ b/CASUAL/LA CHO/ENRIQUEZ, ANABEL ORTEGA.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dole-pc\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA CHO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA CHO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1B208B-2785-450E-A793-319874518FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <definedName name="BALANCE_1">Table1[[#Headers],[BALANCE]]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Sheet1!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="86">
   <si>
     <t>PERIOD</t>
   </si>
@@ -290,12 +289,15 @@
   </si>
   <si>
     <t>11/23,24/2023</t>
+  </si>
+  <si>
+    <t>TOTAL LEAVE BALANCE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -983,7 +985,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1026,7 +1028,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1090,7 +1092,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1150,7 +1152,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1216,7 +1218,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1279,7 +1281,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1377,7 +1379,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1436,7 +1438,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1501,7 +1503,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1544,7 +1546,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1619,7 +1621,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1805,7 +1807,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1871,7 +1873,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1929,7 +1931,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1995,7 +1997,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2051,7 +2053,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2126,7 +2128,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2169,7 +2171,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2235,7 +2237,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2291,7 +2293,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2370,7 +2372,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -2387,25 +2389,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A8:K140" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K140" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2712,7 +2714,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2722,7 +2724,7 @@
       <selection activeCell="Z62" sqref="Z62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2730,34 +2732,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3696" topLeftCell="A65" activePane="bottomLeft"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3690" topLeftCell="A65" activePane="bottomLeft"/>
       <selection activeCell="F4" sqref="F4:G4"/>
-      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
+      <selection pane="bottomLeft" activeCell="C80" sqref="C80:C81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -2778,7 +2780,7 @@
       <c r="J2" s="52"/>
       <c r="K2" s="53"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -2798,7 +2800,7 @@
       <c r="J3" s="54"/>
       <c r="K3" s="55"/>
     </row>
-    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -2820,7 +2822,7 @@
       <c r="J4" s="52"/>
       <c r="K4" s="53"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -2828,7 +2830,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -2841,7 +2843,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="50" t="s">
@@ -2858,7 +2860,7 @@
       <c r="J7" s="50"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -2893,7 +2895,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -2902,7 +2904,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>33.800999999999995</v>
+        <v>35.050999999999995</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -2912,12 +2914,12 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</f>
-        <v>49.25</v>
+        <v>50.5</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>45</v>
       </c>
@@ -2939,7 +2941,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="40">
         <v>43647</v>
       </c>
@@ -2959,7 +2961,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="40">
         <v>43678</v>
       </c>
@@ -2979,7 +2981,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <v>43709</v>
       </c>
@@ -2999,7 +3001,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>43739</v>
       </c>
@@ -3019,7 +3021,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="40">
         <v>43770</v>
       </c>
@@ -3039,7 +3041,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="40">
         <v>43800</v>
       </c>
@@ -3059,7 +3061,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
         <v>46</v>
       </c>
@@ -3077,7 +3079,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="40">
         <v>43831</v>
       </c>
@@ -3097,7 +3099,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="40">
         <v>43862</v>
       </c>
@@ -3117,7 +3119,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="40">
         <v>43891</v>
       </c>
@@ -3143,7 +3145,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="40">
         <v>43922</v>
       </c>
@@ -3163,7 +3165,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="40">
         <v>43952</v>
       </c>
@@ -3183,7 +3185,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="40">
         <v>43983</v>
       </c>
@@ -3203,7 +3205,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="40">
         <v>44013</v>
       </c>
@@ -3223,7 +3225,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="40">
         <v>44044</v>
       </c>
@@ -3243,7 +3245,7 @@
       <c r="J25" s="11"/>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="40">
         <v>44075</v>
       </c>
@@ -3263,7 +3265,7 @@
       <c r="J26" s="11"/>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="40">
         <v>44105</v>
       </c>
@@ -3283,7 +3285,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="40">
         <v>44136</v>
       </c>
@@ -3303,7 +3305,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="40">
         <v>44166</v>
       </c>
@@ -3327,7 +3329,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="48" t="s">
         <v>50</v>
       </c>
@@ -3345,7 +3347,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="40">
         <v>44197</v>
       </c>
@@ -3365,7 +3367,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="40">
         <v>44228</v>
       </c>
@@ -3391,7 +3393,7 @@
         <v>44241</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="40"/>
       <c r="B33" s="20" t="s">
         <v>51</v>
@@ -3413,7 +3415,7 @@
         <v>44250</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="40">
         <v>44256</v>
       </c>
@@ -3439,7 +3441,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="40">
         <v>44287</v>
       </c>
@@ -3459,7 +3461,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="40">
         <v>44317</v>
       </c>
@@ -3479,7 +3481,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="40">
         <v>44348</v>
       </c>
@@ -3499,7 +3501,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="40">
         <v>44378</v>
       </c>
@@ -3519,7 +3521,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="40">
         <v>44409</v>
       </c>
@@ -3539,7 +3541,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="40">
         <v>44440</v>
       </c>
@@ -3559,7 +3561,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="40">
         <v>44470</v>
       </c>
@@ -3579,7 +3581,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="40">
         <v>44501</v>
       </c>
@@ -3599,7 +3601,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="40">
         <v>44531</v>
       </c>
@@ -3623,7 +3625,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="48" t="s">
         <v>55</v>
       </c>
@@ -3641,7 +3643,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="40">
         <v>44562</v>
       </c>
@@ -3665,7 +3667,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="40">
         <v>44593</v>
       </c>
@@ -3685,7 +3687,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="40">
         <v>44621</v>
       </c>
@@ -3705,7 +3707,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="40">
         <v>44652</v>
       </c>
@@ -3729,7 +3731,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="40">
         <v>44682</v>
       </c>
@@ -3753,7 +3755,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="40">
         <v>44713</v>
       </c>
@@ -3779,7 +3781,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="40"/>
       <c r="B51" s="20" t="s">
         <v>78</v>
@@ -3801,7 +3803,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="40"/>
       <c r="B52" s="20" t="s">
         <v>80</v>
@@ -3821,7 +3823,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="40">
         <v>44743</v>
       </c>
@@ -3845,7 +3847,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="40"/>
       <c r="B54" s="20" t="s">
         <v>75</v>
@@ -3867,7 +3869,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="40"/>
       <c r="B55" s="20" t="s">
         <v>77</v>
@@ -3887,7 +3889,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="40">
         <v>44774</v>
       </c>
@@ -3911,7 +3913,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="40">
         <v>44805</v>
       </c>
@@ -3937,7 +3939,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="40"/>
       <c r="B58" s="20" t="s">
         <v>71</v>
@@ -3959,7 +3961,7 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="40"/>
       <c r="B59" s="20" t="s">
         <v>73</v>
@@ -3979,7 +3981,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="49"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="40">
         <v>44835</v>
       </c>
@@ -4005,7 +4007,7 @@
         <v>44862</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="40"/>
       <c r="B61" s="20" t="s">
         <v>72</v>
@@ -4025,7 +4027,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="49"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="40">
         <v>44866</v>
       </c>
@@ -4049,7 +4051,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="40">
         <v>44896</v>
       </c>
@@ -4075,7 +4077,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="40"/>
       <c r="B64" s="20" t="s">
         <v>69</v>
@@ -4095,7 +4097,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="48" t="s">
         <v>64</v>
       </c>
@@ -4113,7 +4115,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="40">
         <v>44927</v>
       </c>
@@ -4139,7 +4141,7 @@
         <v>44931</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="40">
         <v>44958</v>
       </c>
@@ -4159,7 +4161,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="40">
         <v>44986</v>
       </c>
@@ -4185,7 +4187,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="40">
         <v>45017</v>
       </c>
@@ -4205,7 +4207,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="40">
         <v>45047</v>
       </c>
@@ -4231,7 +4233,7 @@
         <v>45076</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="40">
         <v>45078</v>
       </c>
@@ -4257,7 +4259,7 @@
         <v>45082</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="40">
         <v>45108</v>
       </c>
@@ -4283,7 +4285,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="40"/>
       <c r="B73" s="20" t="s">
         <v>67</v>
@@ -4303,7 +4305,7 @@
         <v>45139</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="40">
         <v>45139</v>
       </c>
@@ -4329,7 +4331,7 @@
         <v>45169</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="40">
         <v>45170</v>
       </c>
@@ -4355,7 +4357,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="40">
         <v>45200</v>
       </c>
@@ -4381,7 +4383,7 @@
         <v>45210</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="40">
         <v>45231</v>
       </c>
@@ -4407,7 +4409,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="40"/>
       <c r="B78" s="20" t="s">
         <v>47</v>
@@ -4429,25 +4431,27 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="40">
         <v>45261</v>
       </c>
       <c r="B79" s="20"/>
-      <c r="C79" s="13"/>
+      <c r="C79" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D79" s="39"/>
       <c r="E79" s="9"/>
       <c r="F79" s="20"/>
-      <c r="G79" s="13" t="str">
-        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G79" s="13">
+        <f>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H79" s="39"/>
       <c r="I79" s="9"/>
       <c r="J79" s="11"/>
       <c r="K79" s="20"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="48" t="s">
         <v>83</v>
       </c>
@@ -4465,7 +4469,7 @@
       <c r="J80" s="11"/>
       <c r="K80" s="20"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="40">
         <v>45292</v>
       </c>
@@ -4483,7 +4487,7 @@
       <c r="J81" s="11"/>
       <c r="K81" s="20"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="40"/>
       <c r="B82" s="20"/>
       <c r="C82" s="13"/>
@@ -4499,7 +4503,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="20"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="40"/>
       <c r="B83" s="20"/>
       <c r="C83" s="13"/>
@@ -4515,7 +4519,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="40"/>
       <c r="B84" s="20"/>
       <c r="C84" s="13"/>
@@ -4531,7 +4535,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="40"/>
       <c r="B85" s="20"/>
       <c r="C85" s="13"/>
@@ -4547,7 +4551,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="40"/>
       <c r="B86" s="20"/>
       <c r="C86" s="13"/>
@@ -4563,7 +4567,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="40"/>
       <c r="B87" s="20"/>
       <c r="C87" s="13"/>
@@ -4579,7 +4583,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="40"/>
       <c r="B88" s="20"/>
       <c r="C88" s="13"/>
@@ -4595,7 +4599,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="40"/>
       <c r="B89" s="20"/>
       <c r="C89" s="13"/>
@@ -4611,7 +4615,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="40"/>
       <c r="B90" s="20"/>
       <c r="C90" s="13"/>
@@ -4627,7 +4631,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="40"/>
       <c r="B91" s="20"/>
       <c r="C91" s="13"/>
@@ -4643,7 +4647,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="40"/>
       <c r="B92" s="20"/>
       <c r="C92" s="13"/>
@@ -4659,7 +4663,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="40"/>
       <c r="B93" s="20"/>
       <c r="C93" s="13"/>
@@ -4675,7 +4679,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="40"/>
       <c r="B94" s="20"/>
       <c r="C94" s="13"/>
@@ -4691,7 +4695,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="40"/>
       <c r="B95" s="20"/>
       <c r="C95" s="13"/>
@@ -4707,7 +4711,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="40"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -4723,7 +4727,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="40"/>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -4739,7 +4743,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="40"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -4755,7 +4759,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="40"/>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -4771,7 +4775,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="40"/>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -4787,7 +4791,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="40"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -4803,7 +4807,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="40"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -4819,7 +4823,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="40"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -4835,7 +4839,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="40"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -4851,7 +4855,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="40"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -4867,7 +4871,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="40"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -4883,7 +4887,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="40"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -4899,7 +4903,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="40"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -4915,7 +4919,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="40"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -4931,7 +4935,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="40"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -4947,7 +4951,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="40"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -4963,7 +4967,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -4979,7 +4983,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -4995,7 +4999,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -5011,7 +5015,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -5027,7 +5031,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -5043,7 +5047,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -5059,7 +5063,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -5075,7 +5079,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -5091,7 +5095,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -5107,7 +5111,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -5123,7 +5127,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -5139,7 +5143,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -5155,7 +5159,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -5171,7 +5175,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -5187,7 +5191,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -5203,7 +5207,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -5219,7 +5223,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="40"/>
       <c r="B128" s="20"/>
       <c r="C128" s="13"/>
@@ -5235,7 +5239,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="40"/>
       <c r="B129" s="20"/>
       <c r="C129" s="13"/>
@@ -5251,7 +5255,7 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="40"/>
       <c r="B130" s="20"/>
       <c r="C130" s="13"/>
@@ -5267,7 +5271,7 @@
       <c r="J130" s="11"/>
       <c r="K130" s="20"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="40"/>
       <c r="B131" s="20"/>
       <c r="C131" s="13"/>
@@ -5283,7 +5287,7 @@
       <c r="J131" s="11"/>
       <c r="K131" s="20"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="40"/>
       <c r="B132" s="20"/>
       <c r="C132" s="13"/>
@@ -5299,7 +5303,7 @@
       <c r="J132" s="11"/>
       <c r="K132" s="20"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="40"/>
       <c r="B133" s="20"/>
       <c r="C133" s="13"/>
@@ -5315,7 +5319,7 @@
       <c r="J133" s="11"/>
       <c r="K133" s="20"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="40"/>
       <c r="B134" s="20"/>
       <c r="C134" s="13"/>
@@ -5331,7 +5335,7 @@
       <c r="J134" s="11"/>
       <c r="K134" s="20"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="40"/>
       <c r="B135" s="20"/>
       <c r="C135" s="13"/>
@@ -5347,7 +5351,7 @@
       <c r="J135" s="11"/>
       <c r="K135" s="20"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="40"/>
       <c r="B136" s="20"/>
       <c r="C136" s="13"/>
@@ -5363,7 +5367,7 @@
       <c r="J136" s="11"/>
       <c r="K136" s="20"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="40"/>
       <c r="B137" s="20"/>
       <c r="C137" s="13"/>
@@ -5379,7 +5383,7 @@
       <c r="J137" s="11"/>
       <c r="K137" s="20"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="40"/>
       <c r="B138" s="20"/>
       <c r="C138" s="13"/>
@@ -5395,7 +5399,7 @@
       <c r="J138" s="11"/>
       <c r="K138" s="20"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="40"/>
       <c r="B139" s="20"/>
       <c r="C139" s="13"/>
@@ -5411,7 +5415,7 @@
       <c r="J139" s="11"/>
       <c r="K139" s="20"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="41"/>
       <c r="B140" s="15"/>
       <c r="C140" s="42"/>
@@ -5442,10 +5446,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5468,28 +5472,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D1" s="58" t="s">
         <v>33</v>
       </c>
@@ -5502,7 +5506,7 @@
       <c r="K1" s="59"/>
       <c r="L1" s="59"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -5531,7 +5535,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="D3" s="11"/>
@@ -5555,17 +5559,20 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>85</v>
+      </c>
       <c r="C6" s="38" t="s">
         <v>28</v>
       </c>
@@ -5586,7 +5593,11 @@
       <c r="K6" s="60"/>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <f>SUM(Sheet1!E9,Sheet1!I9)</f>
+        <v>85.550999999999988</v>
+      </c>
       <c r="C7" s="37">
         <v>1</v>
       </c>
@@ -5613,7 +5624,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -5639,7 +5650,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -5665,7 +5676,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -5691,7 +5702,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -5717,7 +5728,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -5743,7 +5754,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -5769,7 +5780,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -5795,7 +5806,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -5815,7 +5826,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -5835,7 +5846,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -5855,7 +5866,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -5876,7 +5887,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -5897,7 +5908,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -5918,7 +5929,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -5939,7 +5950,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -5960,7 +5971,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -5981,7 +5992,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -6002,7 +6013,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -6023,7 +6034,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -6044,7 +6055,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -6065,7 +6076,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -6086,7 +6097,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -6107,7 +6118,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -6128,7 +6139,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -6149,7 +6160,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -6170,7 +6181,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -6191,7 +6202,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -6212,7 +6223,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -6233,7 +6244,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -6254,7 +6265,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -6275,7 +6286,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -6284,7 +6295,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -6293,7 +6304,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -6302,7 +6313,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -6311,7 +6322,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -6320,7 +6331,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -6329,7 +6340,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -6338,7 +6349,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -6347,7 +6358,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -6356,7 +6367,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -6365,7 +6376,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -6374,7 +6385,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -6383,7 +6394,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -6392,7 +6403,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -6401,7 +6412,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -6410,7 +6421,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -6419,7 +6430,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -6428,7 +6439,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -6437,7 +6448,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -6446,7 +6457,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -6455,7 +6466,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -6464,7 +6475,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -6473,7 +6484,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -6482,7 +6493,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -6491,7 +6502,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -6500,7 +6511,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -6509,7 +6520,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -6518,7 +6529,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -6527,7 +6538,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -6536,7 +6547,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>